<commit_message>
update 3-tier arch diagram and efforts
</commit_message>
<xml_diff>
--- a/Design document/efforts-design.xlsx
+++ b/Design document/efforts-design.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\Design document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72EC4E34-9CBD-47A4-99FC-862AA429A83A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Matteo</t>
   </si>
@@ -58,12 +52,21 @@
   </si>
   <si>
     <t>Component diagram</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Overview + Components</t>
+  </si>
+  <si>
+    <t>Overview</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -195,48 +198,57 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -245,15 +257,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,7 +564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -571,176 +574,194 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="27.5">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
-      <c r="A4" s="6">
+    <row r="4" spans="1:3" ht="29">
+      <c r="A4" s="4">
         <v>43788</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>43789</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <f>SUM(C4:C6)</f>
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:3" ht="27">
-      <c r="A9" s="15" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" ht="27.5">
+      <c r="A9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="9">
         <f>SUM(C12:C14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="27">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:3" ht="27.5">
+      <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
     </row>
     <row r="18" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
+      <c r="A20" s="4">
+        <v>43786</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
+      <c r="A21" s="4">
+        <v>43788</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="4">
+        <v>43789</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="10" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="9">
         <f>SUM(C20:C22)</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix requirements and rasd
</commit_message>
<xml_diff>
--- a/Design document/efforts-design.xlsx
+++ b/Design document/efforts-design.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\Design document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C56D93-F066-4413-B812-70C36C74AD72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Matteo</t>
   </si>
@@ -73,12 +67,15 @@
   </si>
   <si>
     <t>Component diagram + Runtime View</t>
+  </si>
+  <si>
+    <t>Fix requirements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -576,28 +573,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27">
+    <row r="1" spans="1:3" ht="27.5">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -620,7 +617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="29">
       <c r="A4" s="4">
         <v>43788</v>
       </c>
@@ -642,7 +639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="4">
         <v>43793</v>
       </c>
@@ -668,7 +665,7 @@
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:3" ht="27">
+    <row r="9" spans="1:3" ht="27.5">
       <c r="A9" s="18" t="s">
         <v>5</v>
       </c>
@@ -716,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="27">
+    <row r="17" spans="1:3" ht="27.5">
       <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
@@ -761,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="45">
+    <row r="22" spans="1:3" ht="29">
       <c r="A22" s="4">
         <v>43789</v>
       </c>
@@ -795,13 +792,24 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="8" t="s">
+      <c r="A25" s="4">
+        <v>43794</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="15"/>
+      <c r="B26" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="9">
-        <f>SUM(C20:C24)</f>
-        <v>8</v>
+      <c r="C26" s="9">
+        <f>SUM(C20:C25)</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -811,5 +819,6 @@
     <mergeCell ref="A17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add component interfaces diagram
</commit_message>
<xml_diff>
--- a/Design document/efforts-design.xlsx
+++ b/Design document/efforts-design.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Desktop\PozziSaccoVentura-SwEng2\Design document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4912E4FC-F68B-4EE0-983C-17C4E0B62C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Matteo</t>
   </si>
@@ -93,12 +87,18 @@
   </si>
   <si>
     <t>Implementation and testing plan</t>
+  </si>
+  <si>
+    <t>Component Interfaces</t>
+  </si>
+  <si>
+    <t>Component Interfaces + Class diagram</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -596,18 +596,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -926,13 +926,35 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="15"/>
-      <c r="B34" s="8" t="s">
+      <c r="A34" s="4">
+        <v>43799</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="6">
         <v>4</v>
       </c>
-      <c r="C34" s="9">
-        <f>SUM(C27:C33)</f>
-        <v>11</v>
+    </row>
+    <row r="35" spans="1:3" ht="29">
+      <c r="A35" s="4">
+        <v>43800</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="15"/>
+      <c r="B36" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="9">
+        <f>SUM(C27:C35)</f>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deployment diagram + various fixes
</commit_message>
<xml_diff>
--- a/Design document/efforts-design.xlsx
+++ b/Design document/efforts-design.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\Design document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662F3602-DEBE-4E72-8C0A-49E79D98A4BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -17,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Matteo</t>
   </si>
@@ -99,12 +103,18 @@
   </si>
   <si>
     <t>UX diagrams</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Deployment + Runtime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -602,28 +612,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27.5">
+    <row r="1" spans="1:3" ht="27">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -646,7 +656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29">
+    <row r="4" spans="1:3" ht="30">
       <c r="A4" s="4">
         <v>43788</v>
       </c>
@@ -668,7 +678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="4">
         <v>43793</v>
       </c>
@@ -702,68 +712,68 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="4">
+        <v>43802</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4">
+        <v>43803</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9">
-        <f>SUM(C4:C8)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="11" spans="1:3" ht="27.5">
-      <c r="A11" s="18" t="s">
+      <c r="C11" s="9">
+        <f>SUM(C4:C10)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" ht="27">
+      <c r="A13" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-    </row>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+    </row>
+    <row r="14" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="4">
-        <v>43783</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="4">
-        <v>43784</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="4">
-        <v>43786</v>
+        <v>43783</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>17</v>
@@ -774,114 +784,114 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4">
+        <v>43784</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4">
+        <v>43786</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4">
         <v>43787</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C19" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29">
-      <c r="A18" s="4">
+    <row r="20" spans="1:3" ht="30">
+      <c r="A20" s="4">
         <v>43795</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="29">
-      <c r="A19" s="4">
-        <v>43796</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A20" s="4">
-        <v>43798</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30">
+      <c r="A21" s="4">
+        <v>43796</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A22" s="4">
+        <v>43798</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="9">
-        <f>SUM(C14:C20)</f>
+      <c r="C24" s="9">
+        <f>SUM(C16:C22)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="27.5">
-      <c r="A24" s="18" t="s">
+    <row r="26" spans="1:3" ht="27">
+      <c r="A26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-    </row>
-    <row r="25" spans="1:3" ht="27.5">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+    </row>
+    <row r="27" spans="1:3" ht="27">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="4">
+    <row r="29" spans="1:3">
+      <c r="A29" s="4">
         <v>43786</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="C27" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="4">
-        <v>43788</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="29">
-      <c r="A29" s="4">
-        <v>43789</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="C29" s="6">
         <v>1</v>
@@ -889,21 +899,21 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="4">
-        <v>43791</v>
+        <v>43788</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C30" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="45">
       <c r="A31" s="4">
-        <v>43793</v>
+        <v>43789</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31" s="6">
         <v>1</v>
@@ -911,21 +921,21 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="4">
-        <v>43794</v>
+        <v>43791</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C32" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4">
-        <v>43797</v>
+        <v>43793</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C33" s="6">
         <v>1</v>
@@ -933,63 +943,85 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4">
-        <v>43799</v>
+        <v>43794</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C34" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="4">
-        <v>43800</v>
+        <v>43797</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C35" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="4">
+        <v>43799</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30">
+      <c r="A37" s="4">
+        <v>43800</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="4">
         <v>43802</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C38" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="4">
+    <row r="39" spans="1:3">
+      <c r="A39" s="4">
         <v>43803</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C39" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="8" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="15"/>
+      <c r="B40" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="9">
-        <f>SUM(C27:C37)</f>
+      <c r="C40" s="9">
+        <f>SUM(C29:C39)</f>
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Paragraph on design decisions
</commit_message>
<xml_diff>
--- a/Design document/efforts-design.xlsx
+++ b/Design document/efforts-design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\Design document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662F3602-DEBE-4E72-8C0A-49E79D98A4BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAF8135-7AA8-4498-A679-F7C39AD670FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
     <t>Deployment</t>
   </si>
   <si>
-    <t>Deployment + Runtime</t>
+    <t>Deployment + Runtime + Design Decisions</t>
   </si>
 </sst>
 </file>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,7 +722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" ht="30">
       <c r="A10" s="4">
         <v>43803</v>
       </c>
@@ -730,7 +730,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -740,7 +740,7 @@
       </c>
       <c r="C11" s="9">
         <f>SUM(C4:C10)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3">

</xml_diff>

<commit_message>
add arch styles and patterns
</commit_message>
<xml_diff>
--- a/Design document/efforts-design.xlsx
+++ b/Design document/efforts-design.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matteo\Desktop\PozziSaccoVentura-SwEng2\Design document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAF8135-7AA8-4498-A679-F7C39AD670FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>Matteo</t>
   </si>
@@ -109,12 +103,15 @@
   </si>
   <si>
     <t>Deployment + Runtime + Design Decisions</t>
+  </si>
+  <si>
+    <t>Architectural styles and patterns</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -612,28 +609,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27">
+    <row r="1" spans="1:3" ht="27.5">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -656,7 +653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="29">
       <c r="A4" s="4">
         <v>43788</v>
       </c>
@@ -678,7 +675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="4">
         <v>43793</v>
       </c>
@@ -722,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="29">
       <c r="A10" s="4">
         <v>43803</v>
       </c>
@@ -748,7 +745,7 @@
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:3" ht="27">
+    <row r="13" spans="1:3" ht="27.5">
       <c r="A13" s="18" t="s">
         <v>5</v>
       </c>
@@ -815,7 +812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30">
+    <row r="20" spans="1:3" ht="29">
       <c r="A20" s="4">
         <v>43795</v>
       </c>
@@ -826,7 +823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30">
+    <row r="21" spans="1:3" ht="29">
       <c r="A21" s="4">
         <v>43796</v>
       </c>
@@ -863,14 +860,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="27">
+    <row r="26" spans="1:3" ht="27.5">
       <c r="A26" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="20"/>
     </row>
-    <row r="27" spans="1:3" ht="27">
+    <row r="27" spans="1:3" ht="27.5">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -908,7 +905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="45">
+    <row r="31" spans="1:3" ht="29">
       <c r="A31" s="4">
         <v>43789</v>
       </c>
@@ -974,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30">
+    <row r="37" spans="1:3" ht="29">
       <c r="A37" s="4">
         <v>43800</v>
       </c>
@@ -1007,14 +1004,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="8" t="s">
+    <row r="40" spans="1:3" ht="29">
+      <c r="A40" s="4">
+        <v>43807</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="6">
         <v>4</v>
       </c>
-      <c r="C40" s="9">
-        <f>SUM(C29:C39)</f>
-        <v>23</v>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="15"/>
+      <c r="B41" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="9">
+        <f>SUM(C29:C40)</f>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>